<commit_message>
Working copy in progress
</commit_message>
<xml_diff>
--- a/analysis/API.xlsx
+++ b/analysis/API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anona\Desktop\Dokumenty\moje\projekty_kod\snyverse\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9853D60D-FFFF-4C3D-944F-27AE39F4346F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC75C41-98E1-4247-8977-5E88D8B29A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,8 +188,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +210,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -359,18 +372,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -389,10 +403,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Správně" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -673,7 +691,7 @@
   <dimension ref="B4:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,19 +706,19 @@
   <sheetData>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -714,61 +732,61 @@
       <c r="F6" s="10"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="1"/>
@@ -777,7 +795,7 @@
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -794,7 +812,7 @@
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -809,7 +827,7 @@
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -822,7 +840,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="4"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -837,10 +855,10 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -855,7 +873,7 @@
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -870,7 +888,7 @@
       <c r="B18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -885,7 +903,7 @@
       <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -900,7 +918,7 @@
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -913,7 +931,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="4"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -931,7 +949,7 @@
       <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -948,7 +966,7 @@
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -963,7 +981,7 @@
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -978,7 +996,7 @@
       <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -993,7 +1011,7 @@
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1008,28 +1026,28 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="4"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="4"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
-      <c r="C30" s="4"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
-      <c r="C31" s="4"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>

</xml_diff>

<commit_message>
Continously making articles api with perzistance layer, tags, categories Updated API and UML
</commit_message>
<xml_diff>
--- a/analysis/API.xlsx
+++ b/analysis/API.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anona\Desktop\Dokumenty\moje\projekty_kod\snyverse\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC75C41-98E1-4247-8977-5E88D8B29A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>PATH</t>
   </si>
@@ -123,9 +122,6 @@
     <t>/articles/delete/{article}</t>
   </si>
   <si>
-    <t>/articles/get/{article}</t>
-  </si>
-  <si>
     <t>/files/create</t>
   </si>
   <si>
@@ -151,12 +147,27 @@
   </si>
   <si>
     <t>only my files</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>CATEGORIES</t>
+  </si>
+  <si>
+    <t>/category/list</t>
+  </si>
+  <si>
+    <t>/articles/{article}</t>
+  </si>
+  <si>
+    <t>/category/{id}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -385,6 +396,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -403,10 +418,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -687,11 +699,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:F31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,10 +714,15 @@
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" customWidth="1"/>
     <col min="6" max="6" width="79.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -722,76 +739,88 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="15" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -807,8 +836,11 @@
       <c r="F11" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
@@ -822,8 +854,11 @@
         <v>18</v>
       </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
@@ -837,24 +872,27 @@
         <v>18</v>
       </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>4</v>
       </c>
@@ -868,8 +906,11 @@
         <v>25</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
@@ -883,8 +924,11 @@
         <v>25</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>2</v>
       </c>
@@ -898,8 +942,11 @@
         <v>25</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
@@ -913,13 +960,16 @@
         <v>10</v>
       </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>25</v>
@@ -928,91 +978,106 @@
         <v>10</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>25</v>
@@ -1021,36 +1086,63 @@
         <v>25</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F31" s="1"/>
+      <c r="G31">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1059,5 +1151,6 @@
     <mergeCell ref="B22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>